<commit_message>
Update beneficial & harmful microbiome list and update readme file
</commit_message>
<xml_diff>
--- a/input/dysbiosis_microbiome_cat.xlsx
+++ b/input/dysbiosis_microbiome_cat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AppData\Roaming\MobaXterm\slash\RemoteFiles\198398_2_26\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AppData\Roaming\MobaXterm\slash\RemoteFiles\65145406_6_40\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9278041-BA49-4040-A896-82E946517F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CB0C4E-F18C-4A73-A9AA-A5208BA560DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52410" yWindow="945" windowWidth="13785" windowHeight="585" xr2:uid="{CC38755F-6577-48FE-A1A7-9F5B9F5D7C0E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{CC38755F-6577-48FE-A1A7-9F5B9F5D7C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>NCBI name</t>
   </si>
@@ -196,6 +196,63 @@
   </si>
   <si>
     <t>s__Clostridioides_difficile</t>
+  </si>
+  <si>
+    <t>Lactobacillus acidophilus</t>
+  </si>
+  <si>
+    <t>s__Lactobacillus_acidophilus</t>
+  </si>
+  <si>
+    <t>Lactobacillus plantarum</t>
+  </si>
+  <si>
+    <t>s__Lactobacillus_plantarum</t>
+  </si>
+  <si>
+    <t>Bifidobacterium animalis</t>
+  </si>
+  <si>
+    <t>s__Bifidobacterium_animalis</t>
+  </si>
+  <si>
+    <t>Lactobacillus reuteri</t>
+  </si>
+  <si>
+    <t>s__Lactobacillus_reuteri</t>
+  </si>
+  <si>
+    <t>Lactobacillus casei</t>
+  </si>
+  <si>
+    <t>s__Lactobacillus_casei</t>
+  </si>
+  <si>
+    <t>Bifidobacterium breve</t>
+  </si>
+  <si>
+    <t>s__Bifidobacterium_breve</t>
+  </si>
+  <si>
+    <t>Bifidobacterium bifidum</t>
+  </si>
+  <si>
+    <t>s__Bifidobacterium_bifidum</t>
+  </si>
+  <si>
+    <t>Streptococcus thermophilus</t>
+  </si>
+  <si>
+    <t>s__Streptococcus_thermophilus</t>
+  </si>
+  <si>
+    <t>Bifidobacterium longum</t>
+  </si>
+  <si>
+    <t>s__Bifidobacterium_longum</t>
+  </si>
+  <si>
+    <t>s__Bifidobacterium_infantis</t>
   </si>
 </sst>
 </file>
@@ -231,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -382,7 +445,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -427,6 +490,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA90404-911C-40EA-B388-AEB4AA02C323}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1089,14 +1155,134 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="38" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>